<commit_message>
Added tools to deal with sizing tkinter windows across different OS and screens, still not finished though.
</commit_message>
<xml_diff>
--- a/Generic_Macro/SavedData/Top50GM2.xlsx
+++ b/Generic_Macro/SavedData/Top50GM2.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B198"/>
+  <dimension ref="A1:B199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2011,7 +2011,7 @@
         <v>44986</v>
       </c>
       <c r="B196" t="n">
-        <v>114975837803218.2</v>
+        <v>114976911118419.2</v>
       </c>
     </row>
     <row r="197">
@@ -2019,7 +2019,7 @@
         <v>45017</v>
       </c>
       <c r="B197" t="n">
-        <v>114659861627124.1</v>
+        <v>114672959226172</v>
       </c>
     </row>
     <row r="198">
@@ -2027,7 +2027,15 @@
         <v>45047</v>
       </c>
       <c r="B198" t="n">
-        <v>112929654879387</v>
+        <v>112917914904701.7</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="3" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B199" t="n">
+        <v>112569394359339.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>